<commit_message>
update crc + Makefile
</commit_message>
<xml_diff>
--- a/MAX7219/docs/matrix_8x8_patterns.xlsx
+++ b/MAX7219/docs/matrix_8x8_patterns.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Pattern_calculator" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="template" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Afficheur" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Afficheur Score" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Feuille5" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="59">
   <si>
     <t xml:space="preserve">C7</t>
   </si>
@@ -152,6 +153,30 @@
   </si>
   <si>
     <t xml:space="preserve">Digit_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATA D7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATA D6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATA D5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATA D4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATA D3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATA D2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATA D1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATA D0</t>
   </si>
   <si>
     <t xml:space="preserve">M0</t>
@@ -372,7 +397,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -489,20 +514,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -532,9 +553,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>89</xdr:col>
-      <xdr:colOff>59400</xdr:colOff>
+      <xdr:colOff>59040</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>108000</xdr:rowOff>
+      <xdr:rowOff>107640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -547,8 +568,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11800080" y="3690720"/>
-          <a:ext cx="4253040" cy="4115160"/>
+          <a:off x="14854680" y="3690720"/>
+          <a:ext cx="5380200" cy="4114800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -564,7 +585,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -574,7 +595,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.66015625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.66"/>
@@ -593,7 +614,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="45" style="0" width="3.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="49" style="0" width="2.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="103" min="51" style="0" width="2.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="104" style="0" width="10.65"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2128,47 +2148,48 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O7" activeCellId="0" sqref="O7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N4" activeCellId="0" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.66015625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="2" style="0" width="2.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="34" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="2.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="3" style="0" width="3.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="11" style="0" width="2.77"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2204,98 +2225,114 @@
       <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="8"/>
+      <c r="C3" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" s="31" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
       <c r="B4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="15"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="31"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="15"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="31"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
       <c r="B6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="15"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="31"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="15"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="31"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1"/>
       <c r="B8" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="15"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="31"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
       <c r="B9" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="15"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="31"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
@@ -2304,14 +2341,14 @@
       <c r="B10" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="32"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="31"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2334,6 +2371,16 @@
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="D3:D10"/>
+    <mergeCell ref="E3:E10"/>
+    <mergeCell ref="F3:F10"/>
+    <mergeCell ref="G3:G10"/>
+    <mergeCell ref="H3:H10"/>
+    <mergeCell ref="I3:I10"/>
+    <mergeCell ref="J3:J10"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2345,7 +2392,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2355,94 +2402,93 @@
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.66015625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="77" min="1" style="0" width="2.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="78" style="0" width="10.65"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D2" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="33"/>
-      <c r="Z2" s="33"/>
-      <c r="AA2" s="33"/>
-      <c r="AB2" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC2" s="33"/>
-      <c r="AD2" s="33"/>
-      <c r="AE2" s="33"/>
-      <c r="AF2" s="33"/>
-      <c r="AG2" s="33"/>
-      <c r="AH2" s="33"/>
-      <c r="AI2" s="33"/>
-      <c r="AJ2" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="AK2" s="33"/>
-      <c r="AL2" s="33"/>
-      <c r="AM2" s="33"/>
-      <c r="AN2" s="33"/>
-      <c r="AO2" s="33"/>
-      <c r="AP2" s="33"/>
-      <c r="AQ2" s="33"/>
-      <c r="AR2" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="AS2" s="33"/>
-      <c r="AT2" s="33"/>
-      <c r="AU2" s="33"/>
-      <c r="AV2" s="33"/>
-      <c r="AW2" s="33"/>
-      <c r="AX2" s="33"/>
-      <c r="AY2" s="33"/>
-      <c r="AZ2" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="BA2" s="33"/>
-      <c r="BB2" s="33"/>
-      <c r="BC2" s="33"/>
-      <c r="BD2" s="33"/>
-      <c r="BE2" s="33"/>
-      <c r="BF2" s="33"/>
-      <c r="BG2" s="33"/>
-      <c r="BH2" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="BI2" s="33"/>
-      <c r="BJ2" s="33"/>
-      <c r="BK2" s="33"/>
-      <c r="BL2" s="33"/>
-      <c r="BM2" s="33"/>
-      <c r="BN2" s="33"/>
-      <c r="BO2" s="33"/>
+      <c r="D2" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="32"/>
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC2" s="32"/>
+      <c r="AD2" s="32"/>
+      <c r="AE2" s="32"/>
+      <c r="AF2" s="32"/>
+      <c r="AG2" s="32"/>
+      <c r="AH2" s="32"/>
+      <c r="AI2" s="32"/>
+      <c r="AJ2" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK2" s="32"/>
+      <c r="AL2" s="32"/>
+      <c r="AM2" s="32"/>
+      <c r="AN2" s="32"/>
+      <c r="AO2" s="32"/>
+      <c r="AP2" s="32"/>
+      <c r="AQ2" s="32"/>
+      <c r="AR2" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS2" s="32"/>
+      <c r="AT2" s="32"/>
+      <c r="AU2" s="32"/>
+      <c r="AV2" s="32"/>
+      <c r="AW2" s="32"/>
+      <c r="AX2" s="32"/>
+      <c r="AY2" s="32"/>
+      <c r="AZ2" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="BA2" s="32"/>
+      <c r="BB2" s="32"/>
+      <c r="BC2" s="32"/>
+      <c r="BD2" s="32"/>
+      <c r="BE2" s="32"/>
+      <c r="BF2" s="32"/>
+      <c r="BG2" s="32"/>
+      <c r="BH2" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="BI2" s="32"/>
+      <c r="BJ2" s="32"/>
+      <c r="BK2" s="32"/>
+      <c r="BL2" s="32"/>
+      <c r="BM2" s="32"/>
+      <c r="BN2" s="32"/>
+      <c r="BO2" s="32"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D3" s="6"/>
@@ -3012,104 +3058,102 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="D1:DD95"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="CC50" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="DA71" activeCellId="0" sqref="DA71"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BV69" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="CL78" activeCellId="0" sqref="CL78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="2.55078125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="99" min="1" style="0" width="2.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="100" min="100" style="0" width="6.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="101" style="0" width="2.55"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D1" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="33"/>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="33"/>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC1" s="33"/>
-      <c r="AD1" s="33"/>
-      <c r="AE1" s="33"/>
-      <c r="AF1" s="33"/>
-      <c r="AG1" s="33"/>
-      <c r="AH1" s="33"/>
-      <c r="AI1" s="33"/>
-      <c r="AJ1" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="AK1" s="33"/>
-      <c r="AL1" s="33"/>
-      <c r="AM1" s="33"/>
-      <c r="AN1" s="33"/>
-      <c r="AO1" s="33"/>
-      <c r="AP1" s="33"/>
-      <c r="AQ1" s="33"/>
-      <c r="AR1" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="AS1" s="33"/>
-      <c r="AT1" s="33"/>
-      <c r="AU1" s="33"/>
-      <c r="AV1" s="33"/>
-      <c r="AW1" s="33"/>
-      <c r="AX1" s="33"/>
-      <c r="AY1" s="33"/>
-      <c r="AZ1" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="BA1" s="33"/>
-      <c r="BB1" s="33"/>
-      <c r="BC1" s="33"/>
-      <c r="BD1" s="33"/>
-      <c r="BE1" s="33"/>
-      <c r="BF1" s="33"/>
-      <c r="BG1" s="33"/>
-      <c r="BH1" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="BI1" s="33"/>
-      <c r="BJ1" s="33"/>
-      <c r="BK1" s="33"/>
-      <c r="BL1" s="33"/>
-      <c r="BM1" s="33"/>
-      <c r="BN1" s="33"/>
-      <c r="BO1" s="33"/>
+      <c r="D1" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="32"/>
+      <c r="AH1" s="32"/>
+      <c r="AI1" s="32"/>
+      <c r="AJ1" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK1" s="32"/>
+      <c r="AL1" s="32"/>
+      <c r="AM1" s="32"/>
+      <c r="AN1" s="32"/>
+      <c r="AO1" s="32"/>
+      <c r="AP1" s="32"/>
+      <c r="AQ1" s="32"/>
+      <c r="AR1" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS1" s="32"/>
+      <c r="AT1" s="32"/>
+      <c r="AU1" s="32"/>
+      <c r="AV1" s="32"/>
+      <c r="AW1" s="32"/>
+      <c r="AX1" s="32"/>
+      <c r="AY1" s="32"/>
+      <c r="AZ1" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="BA1" s="32"/>
+      <c r="BB1" s="32"/>
+      <c r="BC1" s="32"/>
+      <c r="BD1" s="32"/>
+      <c r="BE1" s="32"/>
+      <c r="BF1" s="32"/>
+      <c r="BG1" s="32"/>
+      <c r="BH1" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="BI1" s="32"/>
+      <c r="BJ1" s="32"/>
+      <c r="BK1" s="32"/>
+      <c r="BL1" s="32"/>
+      <c r="BM1" s="32"/>
+      <c r="BN1" s="32"/>
+      <c r="BO1" s="32"/>
     </row>
     <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D2" s="6"/>
@@ -3641,16 +3685,16 @@
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D20" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="33"/>
+      <c r="D20" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="6"/>
@@ -3905,16 +3949,16 @@
       <c r="K28" s="22"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D34" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="E34" s="33"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="33"/>
-      <c r="I34" s="33"/>
-      <c r="J34" s="33"/>
-      <c r="K34" s="33"/>
+      <c r="D34" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="32"/>
+      <c r="J34" s="32"/>
+      <c r="K34" s="32"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D35" s="6"/>
@@ -4689,86 +4733,86 @@
       <c r="AX50" s="22"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="U59" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="V59" s="33"/>
-      <c r="W59" s="33"/>
-      <c r="X59" s="33"/>
-      <c r="Y59" s="33"/>
-      <c r="Z59" s="33"/>
-      <c r="AA59" s="33"/>
-      <c r="AB59" s="33"/>
-      <c r="AC59" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD59" s="33"/>
-      <c r="AE59" s="33"/>
-      <c r="AF59" s="33"/>
-      <c r="AG59" s="33"/>
-      <c r="AH59" s="33"/>
-      <c r="AI59" s="33"/>
-      <c r="AJ59" s="33"/>
-      <c r="AK59" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="AL59" s="33"/>
-      <c r="AM59" s="33"/>
-      <c r="AN59" s="33"/>
-      <c r="AO59" s="33"/>
-      <c r="AP59" s="33"/>
-      <c r="AQ59" s="33"/>
-      <c r="AR59" s="33"/>
-      <c r="AS59" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="AT59" s="33"/>
-      <c r="AU59" s="33"/>
-      <c r="AV59" s="33"/>
-      <c r="AW59" s="33"/>
-      <c r="AX59" s="33"/>
-      <c r="AY59" s="33"/>
-      <c r="AZ59" s="33"/>
-      <c r="BA59" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="BB59" s="33"/>
-      <c r="BC59" s="33"/>
-      <c r="BD59" s="33"/>
-      <c r="BE59" s="33"/>
-      <c r="BF59" s="33"/>
-      <c r="BG59" s="33"/>
-      <c r="BH59" s="33"/>
-      <c r="BI59" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="BJ59" s="33"/>
-      <c r="BK59" s="33"/>
-      <c r="BL59" s="33"/>
-      <c r="BM59" s="33"/>
-      <c r="BN59" s="33"/>
-      <c r="BO59" s="33"/>
-      <c r="BP59" s="33"/>
-      <c r="BQ59" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="BR59" s="33"/>
-      <c r="BS59" s="33"/>
-      <c r="BT59" s="33"/>
-      <c r="BU59" s="33"/>
-      <c r="BV59" s="33"/>
-      <c r="BW59" s="33"/>
-      <c r="BX59" s="33"/>
-      <c r="BY59" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="BZ59" s="33"/>
-      <c r="CA59" s="33"/>
-      <c r="CB59" s="33"/>
-      <c r="CC59" s="33"/>
-      <c r="CD59" s="33"/>
-      <c r="CE59" s="33"/>
-      <c r="CF59" s="33"/>
+      <c r="U59" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="V59" s="32"/>
+      <c r="W59" s="32"/>
+      <c r="X59" s="32"/>
+      <c r="Y59" s="32"/>
+      <c r="Z59" s="32"/>
+      <c r="AA59" s="32"/>
+      <c r="AB59" s="32"/>
+      <c r="AC59" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD59" s="32"/>
+      <c r="AE59" s="32"/>
+      <c r="AF59" s="32"/>
+      <c r="AG59" s="32"/>
+      <c r="AH59" s="32"/>
+      <c r="AI59" s="32"/>
+      <c r="AJ59" s="32"/>
+      <c r="AK59" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL59" s="32"/>
+      <c r="AM59" s="32"/>
+      <c r="AN59" s="32"/>
+      <c r="AO59" s="32"/>
+      <c r="AP59" s="32"/>
+      <c r="AQ59" s="32"/>
+      <c r="AR59" s="32"/>
+      <c r="AS59" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="AT59" s="32"/>
+      <c r="AU59" s="32"/>
+      <c r="AV59" s="32"/>
+      <c r="AW59" s="32"/>
+      <c r="AX59" s="32"/>
+      <c r="AY59" s="32"/>
+      <c r="AZ59" s="32"/>
+      <c r="BA59" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="BB59" s="32"/>
+      <c r="BC59" s="32"/>
+      <c r="BD59" s="32"/>
+      <c r="BE59" s="32"/>
+      <c r="BF59" s="32"/>
+      <c r="BG59" s="32"/>
+      <c r="BH59" s="32"/>
+      <c r="BI59" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="BJ59" s="32"/>
+      <c r="BK59" s="32"/>
+      <c r="BL59" s="32"/>
+      <c r="BM59" s="32"/>
+      <c r="BN59" s="32"/>
+      <c r="BO59" s="32"/>
+      <c r="BP59" s="32"/>
+      <c r="BQ59" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="BR59" s="32"/>
+      <c r="BS59" s="32"/>
+      <c r="BT59" s="32"/>
+      <c r="BU59" s="32"/>
+      <c r="BV59" s="32"/>
+      <c r="BW59" s="32"/>
+      <c r="BX59" s="32"/>
+      <c r="BY59" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="BZ59" s="32"/>
+      <c r="CA59" s="32"/>
+      <c r="CB59" s="32"/>
+      <c r="CC59" s="32"/>
+      <c r="CD59" s="32"/>
+      <c r="CE59" s="32"/>
+      <c r="CF59" s="32"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U60" s="6"/>
@@ -6191,4 +6235,27 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>